<commit_message>
migration added with db restraunt setup
</commit_message>
<xml_diff>
--- a/food_app/data/restaurant_data.xlsx
+++ b/food_app/data/restaurant_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luvam\Downloads\db_assignment\food_app\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luvam\Downloads\db_assignment\food_app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{546309EE-3CD8-4652-8D1A-06454FE3A530}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B63A6C29-9B9C-4A51-B910-F10633DA4CD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6274C7F5-564B-4792-A867-C610112043B4}"/>
   </bookViews>
@@ -805,7 +805,7 @@
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1621,9 +1621,6 @@
       <c r="F31" t="s">
         <v>131</v>
       </c>
-      <c r="G31">
-        <v>18003043388</v>
-      </c>
       <c r="I31" t="s">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
added non relational db connection
</commit_message>
<xml_diff>
--- a/food_app/data/restaurant_data.xlsx
+++ b/food_app/data/restaurant_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luvam\Downloads\db_assignment\food_app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B63A6C29-9B9C-4A51-B910-F10633DA4CD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4AA512F-179A-4815-9C43-263A95E4DC52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6274C7F5-564B-4792-A867-C610112043B4}"/>
   </bookViews>
@@ -19,15 +19,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -804,8 +795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DCEDBB1-0E8F-4893-A7E0-59A20E2A651A}">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
order creation working (re-populate restaurants)
</commit_message>
<xml_diff>
--- a/food_app/data/restaurant_data.xlsx
+++ b/food_app/data/restaurant_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luvam\Downloads\db_assignment\food_app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD603EF-9DF2-4A1E-AD9D-C6788C87595A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{690A1E5B-305E-496A-8AF1-D9EA7FC5235E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6274C7F5-564B-4792-A867-C610112043B4}"/>
+    <workbookView xWindow="5232" yWindow="2628" windowWidth="17280" windowHeight="8880" xr2:uid="{6274C7F5-564B-4792-A867-C610112043B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="133">
   <si>
     <t>rid</t>
   </si>
@@ -60,9 +60,6 @@
     <t>Bar, American, Italian, Vegetarian Friendly</t>
   </si>
   <si>
-    <t>11:30 AM -12:00 AM</t>
-  </si>
-  <si>
     <t>Monday, Wednesday - Sunday</t>
   </si>
   <si>
@@ -162,9 +159,6 @@
     <t>Modern European, French</t>
   </si>
   <si>
-    <t>Monday -Sunday</t>
-  </si>
-  <si>
     <t>9 Raffles Blvd #01-79/80 Millenia Walk Singapore (039596)</t>
   </si>
   <si>
@@ -427,6 +421,9 @@
   </si>
   <si>
     <t>$</t>
+  </si>
+  <si>
+    <t>11:30 AM-12:00 AM</t>
   </si>
 </sst>
 </file>
@@ -801,8 +798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DCEDBB1-0E8F-4893-A7E0-59A20E2A651A}">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -839,7 +836,7 @@
         <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -853,19 +850,19 @@
         <v>10</v>
       </c>
       <c r="D2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
       <c r="F2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G2">
         <v>63415167</v>
       </c>
       <c r="I2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="J2">
         <v>1000</v>
@@ -876,25 +873,25 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
       <c r="D3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G3">
         <v>88798765</v>
       </c>
       <c r="I3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J3">
         <v>1001</v>
@@ -905,25 +902,25 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
         <v>18</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="D4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="G4">
         <v>85183763</v>
       </c>
       <c r="I4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J4">
         <v>1002</v>
@@ -934,25 +931,25 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
         <v>24</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" t="s">
         <v>25</v>
       </c>
-      <c r="D5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>26</v>
-      </c>
-      <c r="F5" t="s">
-        <v>27</v>
       </c>
       <c r="G5">
         <v>94317613</v>
       </c>
       <c r="I5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J5">
         <v>1003</v>
@@ -963,25 +960,25 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" t="s">
         <v>28</v>
-      </c>
-      <c r="C6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" t="s">
-        <v>29</v>
       </c>
       <c r="G6">
         <v>62620238</v>
       </c>
       <c r="I6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J6">
         <v>1004</v>
@@ -992,25 +989,25 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
         <v>31</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" t="s">
         <v>32</v>
-      </c>
-      <c r="D7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" t="s">
-        <v>33</v>
       </c>
       <c r="G7">
         <v>67388818</v>
       </c>
       <c r="I7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J7">
         <v>1005</v>
@@ -1021,25 +1018,25 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" t="s">
         <v>34</v>
       </c>
-      <c r="C8" t="s">
-        <v>35</v>
-      </c>
       <c r="D8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" t="s">
         <v>40</v>
-      </c>
-      <c r="E8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" t="s">
-        <v>41</v>
       </c>
       <c r="G8">
         <v>68183333</v>
       </c>
       <c r="I8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J8">
         <v>1006</v>
@@ -1050,25 +1047,25 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" t="s">
         <v>43</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" t="s">
         <v>44</v>
-      </c>
-      <c r="D9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E9" t="s">
-        <v>45</v>
-      </c>
-      <c r="F9" t="s">
-        <v>46</v>
       </c>
       <c r="G9">
         <v>92303628</v>
       </c>
       <c r="I9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J9">
         <v>1007</v>
@@ -1079,25 +1076,25 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" t="s">
         <v>47</v>
-      </c>
-      <c r="C10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D10" t="s">
-        <v>36</v>
-      </c>
-      <c r="E10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" t="s">
-        <v>49</v>
       </c>
       <c r="G10">
         <v>88421127</v>
       </c>
       <c r="I10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J10">
         <v>1008</v>
@@ -1108,25 +1105,25 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" t="s">
         <v>50</v>
       </c>
-      <c r="C11" t="s">
-        <v>51</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" t="s">
         <v>52</v>
-      </c>
-      <c r="E11" t="s">
-        <v>26</v>
-      </c>
-      <c r="F11" t="s">
-        <v>54</v>
       </c>
       <c r="G11">
         <v>94601960</v>
       </c>
       <c r="I11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J11">
         <v>1009</v>
@@ -1137,25 +1134,25 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" t="s">
         <v>55</v>
       </c>
-      <c r="C12" t="s">
+      <c r="E12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" t="s">
         <v>56</v>
-      </c>
-      <c r="D12" t="s">
-        <v>57</v>
-      </c>
-      <c r="E12" t="s">
-        <v>16</v>
-      </c>
-      <c r="F12" t="s">
-        <v>58</v>
       </c>
       <c r="G12">
         <v>81325248</v>
       </c>
       <c r="I12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J12">
         <v>1010</v>
@@ -1166,28 +1163,28 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" t="s">
         <v>59</v>
       </c>
-      <c r="C13" t="s">
-        <v>61</v>
-      </c>
       <c r="D13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G13">
         <v>62751002</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J13">
         <v>1011</v>
@@ -1198,25 +1195,25 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" t="s">
         <v>64</v>
       </c>
-      <c r="C14" t="s">
+      <c r="E14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" t="s">
         <v>65</v>
-      </c>
-      <c r="D14" t="s">
-        <v>66</v>
-      </c>
-      <c r="E14" t="s">
-        <v>16</v>
-      </c>
-      <c r="F14" t="s">
-        <v>67</v>
       </c>
       <c r="G14">
         <v>62227377</v>
       </c>
       <c r="I14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J14">
         <v>1012</v>
@@ -1227,25 +1224,25 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15" t="s">
+        <v>67</v>
+      </c>
+      <c r="D15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" t="s">
         <v>68</v>
-      </c>
-      <c r="C15" t="s">
-        <v>69</v>
-      </c>
-      <c r="D15" t="s">
-        <v>36</v>
-      </c>
-      <c r="E15" t="s">
-        <v>16</v>
-      </c>
-      <c r="F15" t="s">
-        <v>70</v>
       </c>
       <c r="G15">
         <v>88131577</v>
       </c>
       <c r="I15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J15">
         <v>1013</v>
@@ -1256,25 +1253,25 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" t="s">
+        <v>70</v>
+      </c>
+      <c r="D16" t="s">
         <v>71</v>
       </c>
-      <c r="C16" t="s">
+      <c r="E16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" t="s">
         <v>72</v>
-      </c>
-      <c r="D16" t="s">
-        <v>73</v>
-      </c>
-      <c r="E16" t="s">
-        <v>12</v>
-      </c>
-      <c r="F16" t="s">
-        <v>74</v>
       </c>
       <c r="G16">
         <v>88316875</v>
       </c>
       <c r="I16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J16">
         <v>1014</v>
@@ -1285,25 +1282,25 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
+        <v>73</v>
+      </c>
+      <c r="C17" t="s">
+        <v>74</v>
+      </c>
+      <c r="D17" t="s">
         <v>75</v>
       </c>
-      <c r="C17" t="s">
+      <c r="E17" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" t="s">
         <v>76</v>
-      </c>
-      <c r="D17" t="s">
-        <v>77</v>
-      </c>
-      <c r="E17" t="s">
-        <v>16</v>
-      </c>
-      <c r="F17" t="s">
-        <v>78</v>
       </c>
       <c r="G17">
         <v>68268240</v>
       </c>
       <c r="I17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J17">
         <v>1015</v>
@@ -1314,25 +1311,25 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18" t="s">
+        <v>78</v>
+      </c>
+      <c r="D18" t="s">
         <v>79</v>
       </c>
-      <c r="C18" t="s">
+      <c r="E18" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18" t="s">
         <v>80</v>
-      </c>
-      <c r="D18" t="s">
-        <v>81</v>
-      </c>
-      <c r="E18" t="s">
-        <v>45</v>
-      </c>
-      <c r="F18" t="s">
-        <v>82</v>
       </c>
       <c r="G18">
         <v>62555744</v>
       </c>
       <c r="I18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J18">
         <v>1016</v>
@@ -1343,25 +1340,25 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
+        <v>81</v>
+      </c>
+      <c r="C19" t="s">
+        <v>82</v>
+      </c>
+      <c r="D19" t="s">
         <v>83</v>
       </c>
-      <c r="C19" t="s">
+      <c r="E19" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" t="s">
         <v>84</v>
-      </c>
-      <c r="D19" t="s">
-        <v>85</v>
-      </c>
-      <c r="E19" t="s">
-        <v>16</v>
-      </c>
-      <c r="F19" t="s">
-        <v>86</v>
       </c>
       <c r="G19">
         <v>67057825</v>
       </c>
       <c r="I19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J19">
         <v>1017</v>
@@ -1372,25 +1369,25 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
+        <v>85</v>
+      </c>
+      <c r="C20" t="s">
+        <v>86</v>
+      </c>
+      <c r="D20" t="s">
         <v>87</v>
       </c>
-      <c r="C20" t="s">
+      <c r="E20" t="s">
+        <v>15</v>
+      </c>
+      <c r="F20" t="s">
         <v>88</v>
-      </c>
-      <c r="D20" t="s">
-        <v>89</v>
-      </c>
-      <c r="E20" t="s">
-        <v>16</v>
-      </c>
-      <c r="F20" t="s">
-        <v>90</v>
       </c>
       <c r="G20">
         <v>67350308</v>
       </c>
       <c r="I20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J20">
         <v>1018</v>
@@ -1401,25 +1398,25 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
+        <v>89</v>
+      </c>
+      <c r="C21" t="s">
+        <v>90</v>
+      </c>
+      <c r="D21" t="s">
         <v>91</v>
       </c>
-      <c r="C21" t="s">
+      <c r="E21" t="s">
         <v>92</v>
       </c>
-      <c r="D21" t="s">
+      <c r="F21" t="s">
         <v>93</v>
-      </c>
-      <c r="E21" t="s">
-        <v>94</v>
-      </c>
-      <c r="F21" t="s">
-        <v>95</v>
       </c>
       <c r="G21">
         <v>88178237</v>
       </c>
       <c r="I21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J21">
         <v>1019</v>
@@ -1430,25 +1427,25 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
+        <v>94</v>
+      </c>
+      <c r="C22" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22" t="s">
+        <v>95</v>
+      </c>
+      <c r="E22" t="s">
+        <v>92</v>
+      </c>
+      <c r="F22" t="s">
         <v>96</v>
-      </c>
-      <c r="C22" t="s">
-        <v>56</v>
-      </c>
-      <c r="D22" t="s">
-        <v>97</v>
-      </c>
-      <c r="E22" t="s">
-        <v>94</v>
-      </c>
-      <c r="F22" t="s">
-        <v>98</v>
       </c>
       <c r="G22">
         <v>87416158</v>
       </c>
       <c r="I22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J22">
         <v>1020</v>
@@ -1459,25 +1456,25 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
+        <v>97</v>
+      </c>
+      <c r="C23" t="s">
+        <v>29</v>
+      </c>
+      <c r="D23" t="s">
+        <v>98</v>
+      </c>
+      <c r="E23" t="s">
+        <v>15</v>
+      </c>
+      <c r="F23" t="s">
         <v>99</v>
-      </c>
-      <c r="C23" t="s">
-        <v>30</v>
-      </c>
-      <c r="D23" t="s">
-        <v>100</v>
-      </c>
-      <c r="E23" t="s">
-        <v>16</v>
-      </c>
-      <c r="F23" t="s">
-        <v>101</v>
       </c>
       <c r="G23">
         <v>88282280</v>
       </c>
       <c r="I23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J23">
         <v>1021</v>
@@ -1488,25 +1485,25 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
+        <v>100</v>
+      </c>
+      <c r="C24" t="s">
+        <v>101</v>
+      </c>
+      <c r="D24" t="s">
+        <v>71</v>
+      </c>
+      <c r="E24" t="s">
+        <v>15</v>
+      </c>
+      <c r="F24" t="s">
         <v>102</v>
       </c>
-      <c r="C24" t="s">
+      <c r="H24" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D24" t="s">
-        <v>73</v>
-      </c>
-      <c r="E24" t="s">
+      <c r="I24" t="s">
         <v>16</v>
-      </c>
-      <c r="F24" t="s">
-        <v>104</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="I24" t="s">
-        <v>17</v>
       </c>
       <c r="J24">
         <v>1022</v>
@@ -1517,28 +1514,28 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
+        <v>104</v>
+      </c>
+      <c r="C25" t="s">
+        <v>105</v>
+      </c>
+      <c r="D25" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="C25" t="s">
+      <c r="E25" t="s">
+        <v>15</v>
+      </c>
+      <c r="F25" t="s">
         <v>107</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="E25" t="s">
-        <v>16</v>
-      </c>
-      <c r="F25" t="s">
-        <v>109</v>
       </c>
       <c r="G25">
         <v>88919298</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="I25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J25">
         <v>1023</v>
@@ -1549,25 +1546,25 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
+        <v>109</v>
+      </c>
+      <c r="C26" t="s">
         <v>111</v>
       </c>
-      <c r="C26" t="s">
-        <v>113</v>
-      </c>
       <c r="D26" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E26" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F26" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G26">
         <v>93855240</v>
       </c>
       <c r="I26" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J26">
         <v>1024</v>
@@ -1578,25 +1575,25 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
+        <v>113</v>
+      </c>
+      <c r="C27" t="s">
+        <v>114</v>
+      </c>
+      <c r="D27" t="s">
         <v>115</v>
       </c>
-      <c r="C27" t="s">
+      <c r="E27" t="s">
+        <v>15</v>
+      </c>
+      <c r="F27" t="s">
         <v>116</v>
-      </c>
-      <c r="D27" t="s">
-        <v>117</v>
-      </c>
-      <c r="E27" t="s">
-        <v>16</v>
-      </c>
-      <c r="F27" t="s">
-        <v>118</v>
       </c>
       <c r="G27">
         <v>80127569</v>
       </c>
       <c r="I27" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J27">
         <v>1025</v>
@@ -1607,25 +1604,25 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
+        <v>117</v>
+      </c>
+      <c r="C28" t="s">
+        <v>118</v>
+      </c>
+      <c r="D28" t="s">
+        <v>51</v>
+      </c>
+      <c r="E28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F28" t="s">
         <v>119</v>
-      </c>
-      <c r="C28" t="s">
-        <v>120</v>
-      </c>
-      <c r="D28" t="s">
-        <v>53</v>
-      </c>
-      <c r="E28" t="s">
-        <v>16</v>
-      </c>
-      <c r="F28" t="s">
-        <v>121</v>
       </c>
       <c r="G28">
         <v>64425180</v>
       </c>
       <c r="I28" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J28">
         <v>1026</v>
@@ -1636,25 +1633,25 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
+        <v>120</v>
+      </c>
+      <c r="C29" t="s">
+        <v>121</v>
+      </c>
+      <c r="D29" t="s">
         <v>122</v>
       </c>
-      <c r="C29" t="s">
+      <c r="E29" t="s">
+        <v>15</v>
+      </c>
+      <c r="F29" t="s">
         <v>123</v>
-      </c>
-      <c r="D29" t="s">
-        <v>124</v>
-      </c>
-      <c r="E29" t="s">
-        <v>16</v>
-      </c>
-      <c r="F29" t="s">
-        <v>125</v>
       </c>
       <c r="G29">
         <v>82028168</v>
       </c>
       <c r="I29" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J29">
         <v>1027</v>
@@ -1665,25 +1662,25 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
+        <v>124</v>
+      </c>
+      <c r="C30" t="s">
+        <v>125</v>
+      </c>
+      <c r="D30" t="s">
         <v>126</v>
       </c>
-      <c r="C30" t="s">
+      <c r="E30" t="s">
+        <v>92</v>
+      </c>
+      <c r="F30" t="s">
         <v>127</v>
-      </c>
-      <c r="D30" t="s">
-        <v>128</v>
-      </c>
-      <c r="E30" t="s">
-        <v>94</v>
-      </c>
-      <c r="F30" t="s">
-        <v>129</v>
       </c>
       <c r="G30">
         <v>96260084</v>
       </c>
       <c r="I30" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J30">
         <v>1028</v>
@@ -1694,22 +1691,22 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D31" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E31" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F31" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="I31" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J31">
         <v>1029</v>

</xml_diff>

<commit_message>
order data and order history added
</commit_message>
<xml_diff>
--- a/food_app/data/restaurant_data.xlsx
+++ b/food_app/data/restaurant_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luvam\Downloads\db_assignment\food_app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{690A1E5B-305E-496A-8AF1-D9EA7FC5235E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AFC65A8-932F-4DE6-A9C9-F777AC5E49E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5232" yWindow="2628" windowWidth="17280" windowHeight="8880" xr2:uid="{6274C7F5-564B-4792-A867-C610112043B4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6274C7F5-564B-4792-A867-C610112043B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -798,8 +798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DCEDBB1-0E8F-4893-A7E0-59A20E2A651A}">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>